<commit_message>
compiles, doesn't run, needs tidying
</commit_message>
<xml_diff>
--- a/scratchpad.xlsx
+++ b/scratchpad.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Who Knows About Who</t>
   </si>
@@ -21,6 +21,9 @@
     <t xml:space="preserve">Data Stores</t>
   </si>
   <si>
+    <t>static</t>
+  </si>
+  <si>
     <t>Map</t>
   </si>
   <si>
@@ -33,6 +36,9 @@
     <t>xy-bool</t>
   </si>
   <si>
+    <t>struct</t>
+  </si>
+  <si>
     <t>XY</t>
   </si>
   <si>
@@ -78,10 +84,19 @@
     <t>xy</t>
   </si>
   <si>
+    <t>dynamic</t>
+  </si>
+  <si>
     <t>EntityComponents</t>
   </si>
   <si>
     <t>component_id-component</t>
+  </si>
+  <si>
+    <t>IComponent</t>
+  </si>
+  <si>
+    <t>Mobility</t>
   </si>
 </sst>
 </file>
@@ -634,18 +649,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.421875"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" width="13.421875"/>
-    <col bestFit="1" min="3" max="3" width="11.00390625"/>
+    <col customWidth="1" min="2" max="2" width="20.421875"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="13.421875"/>
+    <col bestFit="1" min="4" max="4" width="11.00390625"/>
     <col bestFit="1" min="6" max="6" width="17.140625"/>
     <col bestFit="1" min="7" max="7" width="32.00390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
       <c r="F1" t="s">
         <v>1</v>
       </c>
@@ -657,103 +672,143 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="F7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>